<commit_message>
Updated Insights of response time adding more points
</commit_message>
<xml_diff>
--- a/excel/FactorialAnalysisBiggerThroughput.xlsx
+++ b/excel/FactorialAnalysisBiggerThroughput.xlsx
@@ -1066,7 +1066,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1684,11 +1684,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="29057238"/>
-        <c:axId val="2121790"/>
+        <c:axId val="83229315"/>
+        <c:axId val="92898516"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="29057238"/>
+        <c:axId val="83229315"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1730,12 +1730,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121790"/>
+        <c:crossAx val="92898516"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121790"/>
+        <c:axId val="92898516"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,7 +1777,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29057238"/>
+        <c:crossAx val="83229315"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1805,7 +1805,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2393,11 +2393,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="70279646"/>
-        <c:axId val="40573280"/>
+        <c:axId val="15811962"/>
+        <c:axId val="32134473"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70279646"/>
+        <c:axId val="15811962"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2439,12 +2439,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40573280"/>
+        <c:crossAx val="32134473"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40573280"/>
+        <c:axId val="32134473"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2486,7 +2486,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70279646"/>
+        <c:crossAx val="15811962"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2525,9 +2525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>211320</xdr:colOff>
+      <xdr:colOff>210960</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2536,7 +2536,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="13495680" y="10067760"/>
-        <a:ext cx="7566480" cy="3303000"/>
+        <a:ext cx="7566120" cy="3302640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2555,9 +2555,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>774360</xdr:colOff>
+      <xdr:colOff>774000</xdr:colOff>
       <xdr:row>161</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2566,7 +2566,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12339360" y="25997040"/>
-        <a:ext cx="7734960" cy="3190320"/>
+        <a:ext cx="7734600" cy="3189960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2587,7 +2587,7 @@
   <dimension ref="B1:AI225"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="F47" activeCellId="0" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>